<commit_message>
Update scenario period and enhance Tableau CSV downloader
- Changed fixed period in EpisodeDeepDiveModule from "Q1 2026" to "Q1 2025".
- Refactored _is_numeric_series to _clean_and_round_series for better handling of numeric-like strings.
- Introduced _try_numeric_for_sort to facilitate numeric-aware sorting.
- Improved detail output sorting in main function.
- Renamed format_match_headers_green to format_match_cells_true_false for clarity.
- Added new script tableau_download_test.py for downloading Tableau view data with multi-select filters.
- Updated mapping_file.xlsx to reflect changes.
</commit_message>
<xml_diff>
--- a/mapping_file.xlsx
+++ b/mapping_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bainandcompany-my.sharepoint.com/personal/priya_dutta_bain_com/Documents/Documents/Ep-DD-wideformat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="92" documentId="13_ncr:1_{A7573781-DE2A-41D2-8F94-1821F323C354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E2764CE-D93B-4260-8C24-6FEBA6C9236B}"/>
+  <xr:revisionPtr revIDLastSave="108" documentId="13_ncr:1_{A7573781-DE2A-41D2-8F94-1821F323C354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D76F2F3-23E1-40FE-9DF8-2DBC88B45B33}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-1965" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dashboard_sheet_column_mapping" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7523" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7528" uniqueCount="541">
   <si>
     <t>live_in_canada</t>
   </si>
@@ -1660,6 +1660,12 @@
   </si>
   <si>
     <t>%_round</t>
+  </si>
+  <si>
+    <t>Alberta|British Columbia|Manitoba / Saskatchewan|Newbrunswick|Newfoundland/Labrador|Northern Territories|Nova Scotia|Ontario|Quebec</t>
+  </si>
+  <si>
+    <t>NPS_prov</t>
   </si>
 </sst>
 </file>
@@ -3225,8 +3231,8 @@
   <dimension ref="A1:I194"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+      <pane ySplit="1" topLeftCell="A138" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O167" sqref="O167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4465,7 +4471,7 @@
         <v>523</v>
       </c>
       <c r="E55" s="21" t="s">
-        <v>523</v>
+        <v>540</v>
       </c>
       <c r="F55" s="20"/>
       <c r="G55" s="20" t="s">
@@ -4840,7 +4846,7 @@
         <v>523</v>
       </c>
       <c r="E72" s="21" t="s">
-        <v>523</v>
+        <v>540</v>
       </c>
       <c r="F72" s="20"/>
       <c r="G72" s="20" t="s">
@@ -6469,7 +6475,7 @@
         <v>523</v>
       </c>
       <c r="E145" s="21" t="s">
-        <v>523</v>
+        <v>540</v>
       </c>
       <c r="F145" s="20"/>
       <c r="G145" s="20"/>
@@ -6495,9 +6501,7 @@
         <v>522</v>
       </c>
       <c r="F146" s="20"/>
-      <c r="G146" s="20" t="s">
-        <v>517</v>
-      </c>
+      <c r="G146" s="20"/>
       <c r="H146" s="20"/>
       <c r="I146" s="20">
         <v>5</v>
@@ -6517,12 +6521,10 @@
         <v>516</v>
       </c>
       <c r="E147" s="21" t="s">
-        <v>516</v>
+        <v>522</v>
       </c>
       <c r="F147" s="20"/>
-      <c r="G147" s="20" t="s">
-        <v>517</v>
-      </c>
+      <c r="G147" s="20"/>
       <c r="H147" s="20"/>
       <c r="I147" s="20"/>
     </row>
@@ -6867,7 +6869,7 @@
         <v>523</v>
       </c>
       <c r="E163" s="21" t="s">
-        <v>523</v>
+        <v>540</v>
       </c>
       <c r="F163" s="20"/>
       <c r="G163" s="20" t="s">
@@ -6915,12 +6917,10 @@
         <v>516</v>
       </c>
       <c r="E165" s="21" t="s">
-        <v>516</v>
+        <v>522</v>
       </c>
       <c r="F165" s="20"/>
-      <c r="G165" s="20" t="s">
-        <v>517</v>
-      </c>
+      <c r="G165" s="20"/>
       <c r="H165" s="20"/>
       <c r="I165" s="20"/>
     </row>
@@ -7595,10 +7595,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58BAAE34-14CB-43F5-950E-C6CD7CBBC8CA}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7621,6 +7621,38 @@
       </c>
       <c r="B2" s="6" t="s">
         <v>534</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>460</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>532</v>
       </c>
     </row>
   </sheetData>
@@ -26470,8 +26502,8 @@
   <dimension ref="A1:I226"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C56" sqref="C56"/>
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E82" sqref="E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -31584,8 +31616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AAAD4B1-5013-4526-A813-4BE345716FD1}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:B21"/>
+    <sheetView showGridLines="0" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>